<commit_message>
Mon Sep 26 15:56:02 CST 2022
</commit_message>
<xml_diff>
--- a/书籍/我的第一本算法书/算法.xlsx
+++ b/书籍/我的第一本算法书/算法.xlsx
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43">
   <si>
     <t>排序算法</t>
   </si>
@@ -292,6 +292,12 @@
   </si>
   <si>
     <t>O(n^2), 优化后为O(m+nlogn)。</t>
+  </si>
+  <si>
+    <t>A* 算法</t>
+  </si>
+  <si>
+    <t>在图中求解最短路径问题的算法，通过预估值计算。比广度优先算法的探索格子要少。预估值：起点到当前探索节点到的步数、当前探索节点到终点的预估值（可以根据各种算法预估，如曼哈顿：横+纵的步数）</t>
   </si>
 </sst>
 </file>
@@ -299,8 +305,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -321,8 +327,113 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -330,29 +441,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -367,30 +456,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -403,67 +470,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -480,49 +486,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -534,133 +612,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -704,11 +710,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -718,6 +745,24 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -739,30 +784,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -771,172 +792,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -954,12 +960,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1288,11 +1288,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="22.3984375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="14.84375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="56.2421875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="61.5859375" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="6"/>
+    <col min="1" max="1" width="22.3984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.84375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="56.2421875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="61.5859375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:4">
@@ -1310,86 +1310,86 @@
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:4">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:4">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:4">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" ht="64" customHeight="1" spans="1:4">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:4">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1463,13 +1463,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.9140625" defaultRowHeight="40" customHeight="1" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="19.9140625" defaultRowHeight="40" customHeight="1" outlineLevelRow="5" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="19.9140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="81.8984375" style="1" customWidth="1"/>
@@ -1528,6 +1528,15 @@
         <v>40</v>
       </c>
     </row>
+    <row r="6" ht="50" customHeight="1" spans="1:3">
+      <c r="A6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>